<commit_message>
geupdate tot US 6
</commit_message>
<xml_diff>
--- a/FO + TO + Test/Test rapportage.xlsx
+++ b/FO + TO + Test/Test rapportage.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="250" documentId="8_{B2706BB1-B7A2-4280-B11F-089947E83C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A966D53-EC08-4456-92AA-E88AB76379CE}"/>
+  <xr:revisionPtr revIDLastSave="315" documentId="8_{B2706BB1-B7A2-4280-B11F-089947E83C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1C21262-9779-4871-84B9-DA008A7D4034}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="141">
   <si>
     <t>NUMMER</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Test resultaat</t>
   </si>
   <si>
-    <t>sprint.user-storie.acceptatiecriteria.test#</t>
-  </si>
-  <si>
     <t>Naam User Storie</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Tijd besteed in minuten</t>
   </si>
   <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
     <t>Het systeem toont een omschrijving van het product.</t>
   </si>
   <si>
@@ -80,19 +74,7 @@
     <t xml:space="preserve">De beschrijving wordt perproduct weergegeven. </t>
   </si>
   <si>
-    <t>1.1.1.2</t>
-  </si>
-  <si>
-    <t>1.1.1.3</t>
-  </si>
-  <si>
     <t>Het systeem toont de prijs van het product.</t>
-  </si>
-  <si>
-    <t>1.1.1.4</t>
-  </si>
-  <si>
-    <t>1.1.1.5</t>
   </si>
   <si>
     <t>Bekijk de productpagina. Zoek naar de prijs.</t>
@@ -130,21 +112,6 @@
     <t>Het systeem toont een link naar filmmateriaal van het product.</t>
   </si>
   <si>
-    <t>1.1.6.1</t>
-  </si>
-  <si>
-    <t>1.1.5.1</t>
-  </si>
-  <si>
-    <t>1.1.4.1</t>
-  </si>
-  <si>
-    <t>1.1.3.1</t>
-  </si>
-  <si>
-    <t>1.1.2.1</t>
-  </si>
-  <si>
     <t>Open producten 16 en 222.</t>
   </si>
   <si>
@@ -185,21 +152,6 @@
     <t>29-9-2022 Jochem</t>
   </si>
   <si>
-    <t>1.2.1.1</t>
-  </si>
-  <si>
-    <t>1.2.2.1</t>
-  </si>
-  <si>
-    <t>1.2.3.1</t>
-  </si>
-  <si>
-    <t>1.2.4.1</t>
-  </si>
-  <si>
-    <t>1.2.5.1</t>
-  </si>
-  <si>
     <t>De beschrijving wordt per 
 product weergegeven.</t>
   </si>
@@ -219,24 +171,6 @@
 Product 222 geeft geen link weer</t>
   </si>
   <si>
-    <t>1.2.6.1</t>
-  </si>
-  <si>
-    <t>2.3.1.1</t>
-  </si>
-  <si>
-    <t>2.3.2.1</t>
-  </si>
-  <si>
-    <t>2.3.3.1</t>
-  </si>
-  <si>
-    <t>2.3.4.1</t>
-  </si>
-  <si>
-    <t>2.3.5.1</t>
-  </si>
-  <si>
     <t>Als bezoeker kan ik zoeken op een productnaam.</t>
   </si>
   <si>
@@ -292,6 +226,240 @@
   </si>
   <si>
     <t>Het systeem sorteert de producten op de ingestelde volgorde. In het geval van optie Prijs aflopend zijn de getoonde producten aflopend in prijs. In het geval van optie Naam oplopend zijn de getoonde producten gesorteerd op alfabetische volgorde.</t>
+  </si>
+  <si>
+    <t>De bezoeker moet een item kunnen toevoegen aan de winkelmand.</t>
+  </si>
+  <si>
+    <t>Druk op de knop “voeg toe aan winkelmand” op een product pagina</t>
+  </si>
+  <si>
+    <t>Het product wordt in de winkelmand geplaatst</t>
+  </si>
+  <si>
+    <t>Het gewenste product zit in de winkelmand</t>
+  </si>
+  <si>
+    <t>Er moet een duidelijk knop zijn voor de winkelmand.</t>
+  </si>
+  <si>
+    <t>Kijk op de pagina naar een knop die naar de winkelmand verwijst</t>
+  </si>
+  <si>
+    <t>Er is een knop zichtbaar</t>
+  </si>
+  <si>
+    <t>Je ziet een knop</t>
+  </si>
+  <si>
+    <t>De bezoeker moet in de winkelmand een overzicht zien van zijn producten.</t>
+  </si>
+  <si>
+    <t>Ga naar de winkel mand en bekijk de pagina.</t>
+  </si>
+  <si>
+    <t>Een lijst met producten zichtbaar</t>
+  </si>
+  <si>
+    <t>Als er items in de winkelmand zitten zijn die zichtbaar</t>
+  </si>
+  <si>
+    <t>De winkelmand moet binnen een seconde laden.</t>
+  </si>
+  <si>
+    <t>Met een stopwatch timen hoe lang het duurt tot dat de pagina geladen is</t>
+  </si>
+  <si>
+    <t>Het laden duurt minder dan een seconde.</t>
+  </si>
+  <si>
+    <t>Het duurt minder dan een seconden.</t>
+  </si>
+  <si>
+    <t>2-12-2022 mees</t>
+  </si>
+  <si>
+    <t>user-storie.acceptatiecriteria.test#</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>1.5.1</t>
+  </si>
+  <si>
+    <t>1.6.1</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>2.3.1</t>
+  </si>
+  <si>
+    <t>2.4.1</t>
+  </si>
+  <si>
+    <t>2.5.1</t>
+  </si>
+  <si>
+    <t>2.6.1</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
+  <si>
+    <t>3.4.1</t>
+  </si>
+  <si>
+    <t>3.5.1</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>5.1.1</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>4.3.1</t>
+  </si>
+  <si>
+    <t>4.4.1</t>
+  </si>
+  <si>
+    <t>De klant moet in de winkelmand alle items zien die hij heeft toegevoegd.</t>
+  </si>
+  <si>
+    <t>Voeg een aantal producten toe aan de winkelmand en ga naar de winkelmand pagina</t>
+  </si>
+  <si>
+    <t>De gewenste producten worden getoond</t>
+  </si>
+  <si>
+    <t>De gewenste producten zitten in de winkelmand</t>
+  </si>
+  <si>
+    <t>De klant moet de prijs van zijn producten kunnen zien.</t>
+  </si>
+  <si>
+    <t>Kijk op de pagina naar de producten en kijk of daar een prijs bij staat</t>
+  </si>
+  <si>
+    <t>De prijs is  per product zichtbaar</t>
+  </si>
+  <si>
+    <t>De prijs is te zien per product</t>
+  </si>
+  <si>
+    <t>De klant moet de totaalprijs kunnen zien.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kijk op de winkelmand pagina of er een totaalprijs zichtbaar is </t>
+  </si>
+  <si>
+    <t>Een aparte sectie met de totaal prijs er in</t>
+  </si>
+  <si>
+    <t>Er is een tabel met de Totaalprijs van alle producten</t>
+  </si>
+  <si>
+    <t>De naam van de producten moet zichtbaar zijn.</t>
+  </si>
+  <si>
+    <t>Kijk op de winkelmand pagina of de producten met een naam zijn aangegeven</t>
+  </si>
+  <si>
+    <t>Elk product heeft een naam</t>
+  </si>
+  <si>
+    <t>De producten zijn met een naam aangegeven</t>
+  </si>
+  <si>
+    <t>5.2.1</t>
+  </si>
+  <si>
+    <t>5.3.1</t>
+  </si>
+  <si>
+    <t>5.4.1</t>
+  </si>
+  <si>
+    <t>De klant moet het aantal producten kunnen aanpassen</t>
+  </si>
+  <si>
+    <t>Pas het aantal Producten aan via de pijltjes of een nieuw aantal typen in het nummer veld en klik op opslaan/enter</t>
+  </si>
+  <si>
+    <t>Het aantal en de prijs worden aangepast naar het bijbehorende aantal</t>
+  </si>
+  <si>
+    <t>De prijs wordt aangepast aan de hand van het aantal</t>
+  </si>
+  <si>
+    <t>Er moet een veld zijn waarin de klant het aantal kan aanpassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kijk of er een veld is met een aantal die aan te passen is </t>
+  </si>
+  <si>
+    <t>Er is een veld zichtbaar om het aantal aan te passen</t>
+  </si>
+  <si>
+    <t>Het veld is zichtbaar</t>
+  </si>
+  <si>
+    <t>Er moet een knop zijn om een item helemaal te verwijderen</t>
+  </si>
+  <si>
+    <t>Klik op de knop “Delete”</t>
+  </si>
+  <si>
+    <t>Het bijbehorende product verdwijnt uit de winkelmand</t>
+  </si>
+  <si>
+    <t>Het product verdwijnt</t>
+  </si>
+  <si>
+    <t>De items moeten binnen een seconde verdwijnen uit de winkelmand.</t>
+  </si>
+  <si>
+    <t>Het laden duurt minder dan een seconde. Het laden duurt minder dan een seconde.</t>
+  </si>
+  <si>
+    <t>Het duurde minder dan een seconde</t>
+  </si>
+  <si>
+    <t>6.1.1</t>
+  </si>
+  <si>
+    <t>6.2.1</t>
+  </si>
+  <si>
+    <t>6.3.1</t>
+  </si>
+  <si>
+    <t>6.4.1</t>
   </si>
 </sst>
 </file>
@@ -304,7 +472,7 @@
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <b/>
       <sz val="11"/>
@@ -493,6 +661,13 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -675,7 +850,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -763,6 +938,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -820,36 +1015,39 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -953,6 +1151,39 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -962,6 +1193,84 @@
         <family val="2"/>
         <scheme val="major"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1010,117 +1319,6 @@
         <family val="2"/>
         <scheme val="major"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1175,13 +1373,17 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Lijst" displayName="Lijst" ref="B3:H26" headerRowDxfId="9" dataDxfId="7" totalsRowDxfId="8">
-  <autoFilter ref="B3:H26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Lijst" displayName="Lijst" ref="B3:H28" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10">
+  <autoFilter ref="B3:H28" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DATUM + NAAM" totalsRowLabel="Totaal" dataDxfId="6" totalsRowDxfId="12" dataCellStyle="Datum"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NUMMER" dataDxfId="5" totalsRowDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TEST NAAM" totalsRowFunction="count" dataDxfId="4" totalsRowDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DATUM + NAAM" totalsRowLabel="Totaal" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Datum"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NUMMER" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TEST NAAM" totalsRowFunction="count" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="4" xr3:uid="{50103B61-6881-4CFA-968E-4B0BE9D7FB43}" name="Test uitvoering" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{C875DA73-AD7F-44E7-8483-520C38701465}" name="Gewenst resultaat" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{FA098F8B-A30B-4AC5-A8A1-698A8B76C077}" name="Test resultaat" dataDxfId="1"/>
@@ -1463,10 +1665,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H26"/>
+  <dimension ref="B1:H39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1493,7 +1695,7 @@
     </row>
     <row r="3" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -1505,413 +1707,664 @@
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <v>44562</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
-        <v>44562</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="6">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="H5" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>31</v>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H6" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>31</v>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H7" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
-        <v>49</v>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H8" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>49</v>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H9" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
-        <v>49</v>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="H10" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="G20" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="9" t="s">
+      <c r="F22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="G22" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="F23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="2" t="s">
+    </row>
+    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="2" t="s">
+    </row>
+    <row r="26" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="2" t="s">
+    </row>
+    <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="F27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="9" t="s">
+    </row>
+    <row r="28" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="F28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="9" t="s">
+    </row>
+    <row r="29" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="8"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="8"/>
+      <c r="C30" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" s="9"/>
+    </row>
+    <row r="31" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="8"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>

</xml_diff>